<commit_message>
Fast and efficient running of semi-supervised CRF, by training the supervised CRF separately and using that CRF to all the semi-supervised iterations.
</commit_message>
<xml_diff>
--- a/docs/results.xlsx
+++ b/docs/results.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="19340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feature Selection" sheetId="1" r:id="rId1"/>
+    <sheet name="Feature Selection Batch CRF" sheetId="2" r:id="rId2"/>
+    <sheet name="Feature Selection Batch CRF Fin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -18,8 +20,26 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="csv.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="MacOSX:Users:david:Downloads:csv.csv" thousands=" " tab="0" space="1" comma="1" consecutive="1">
+      <textFields count="7">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>R</t>
   </si>
@@ -39,13 +59,19 @@
     <t>P</t>
   </si>
   <si>
-    <t>DIF</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Iterations</t>
+    <t>CRF Iterations</t>
+  </si>
+  <si>
+    <t>DIF MAX</t>
+  </si>
+  <si>
+    <t>DIF 100%</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -55,7 +81,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,6 +121,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -113,7 +146,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,29 +158,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,8 +440,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="613032824"/>
-        <c:axId val="688062248"/>
+        <c:axId val="679339400"/>
+        <c:axId val="679342616"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -417,9 +460,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'Feature Selection'!$A$3:$A$14</c:f>
@@ -522,8 +562,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="613032824"/>
-        <c:axId val="688062248"/>
+        <c:axId val="679339400"/>
+        <c:axId val="679342616"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -542,9 +582,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:cat>
             <c:numRef>
               <c:f>'Feature Selection'!$A$3:$A$14</c:f>
@@ -597,31 +634,31 @@
                 <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.00312358796296296</c:v>
+                  <c:v>0.00297550925925926</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00345898148148148</c:v>
+                  <c:v>0.00298123842592592</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00972633101851851</c:v>
+                  <c:v>0.00839125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0120942013888889</c:v>
+                  <c:v>0.0115028009259259</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0129257638888889</c:v>
+                  <c:v>0.0131295138888889</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0123128935185185</c:v>
+                  <c:v>0.0115464351851852</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0118163657407407</c:v>
+                  <c:v>0.0101717476851852</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0116846875</c:v>
+                  <c:v>0.0103472453703704</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0122857175925926</c:v>
+                  <c:v>0.0108697222222222</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.00940233796296296</c:v>
@@ -647,11 +684,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="820458744"/>
-        <c:axId val="569934840"/>
+        <c:axId val="679348552"/>
+        <c:axId val="679345480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="613032824"/>
+        <c:axId val="679339400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="688062248"/>
+        <c:crossAx val="679342616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -669,9 +706,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="688062248"/>
+        <c:axId val="679342616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -680,12 +718,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="613032824"/>
+        <c:crossAx val="679339400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="569934840"/>
+        <c:axId val="679345480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -695,12 +733,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="820458744"/>
+        <c:crossAx val="679348552"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="820458744"/>
+        <c:axId val="679348552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +748,947 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569934840"/>
+        <c:crossAx val="679345480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRF Iterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection'!$G$3:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>273.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>293.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>276.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>262.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>271.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>198.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>226.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>203.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="679432168"/>
+        <c:axId val="679428888"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection'!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.00297550925925926</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00298123842592592</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00839125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0115028009259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0131295138888889</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0115464351851852</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0101717476851852</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0103472453703704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0108697222222222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00940233796296296</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00977797453703703</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00915353009259259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="679422792"/>
+        <c:axId val="679425864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="679422792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="679425864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="679425864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="679422792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="679428888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="679432168"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="679432168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="679428888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.630025247620897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.701828681424447</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.713359273670558</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.720775623268698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.723654283548143</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.726022304832714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.722395165720564</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.716488300380918</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.720212961263081</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.726390922401171</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.721222040370977</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.723373318793166</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.537798408488064</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.604442970822281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.638262599469496</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.647049071618037</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.632957559681698</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.647546419098143</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.654011936339523</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.654840848806366</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.650364721485411</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.657990716180371</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.657493368700265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.659814323607427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="678560232"/>
+        <c:axId val="678557000"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$E$3:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.580270101064306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.649505656007838</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.673724735322425</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.681925395300079</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.675274142200212</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.684542586750789</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.686504829026364</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68427890861845</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.683509016464849</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.690501043841336</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.687884832191484</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.69013351829374</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="678560232"/>
+        <c:axId val="678557000"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.00132328703703704</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00365015046296296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00481372685185185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00635143518518518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00278131944444444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00534872685185185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00717331018518518</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00607599537037037</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00551784722222222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00701650462962963</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00627563657407407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00792707175925926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="678551080"/>
+        <c:axId val="678554136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="678560232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678557000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="678557000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678560232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="678554136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678551080"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="678551080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678554136"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -731,7 +1709,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1200"/>
+        <a:defRPr sz="1400"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -744,20 +1722,1317 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRF Iterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$G$3:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>213.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>281.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>101.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>222.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>297.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>249.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>282.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>332.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="678514904"/>
+        <c:axId val="678518168"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF'!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.00132328703703704</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00365015046296296</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00481372685185185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00635143518518518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00278131944444444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00534872685185185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00717331018518518</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00607599537037037</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00551784722222222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00701650462962963</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00627563657407407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00792707175925926</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="678524280"/>
+        <c:axId val="678521192"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="678524280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678521192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="678521192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678524280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="678518168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678514904"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="678514904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="678518168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>P</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$C$3:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.644159072</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.700251402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.709767442</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.711241734</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.720913108</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.723040118</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.728529303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.714130828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.730410448</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.727675276752768</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.719291907514451</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.718231047</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$D$3:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.515583554</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.600298408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.632460212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.641909814</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.649204244</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.651359416</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.655338196</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.655172414</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.649038462</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.653846153846154</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.660145888594164</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.659648541</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="602453896"/>
+        <c:axId val="112410248"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>F1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$E$3:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.572744015</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.646433991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.668887525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.674799582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.683182135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.685330542</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.689998254</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.683382328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.687324438</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.688787984631505</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.688450899031812</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.687694435</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="602453896"/>
+        <c:axId val="112410248"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.00146412037037037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00226041666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00227893518518518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00340509259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00409953703703704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00388541666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00425231481481481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00234259259259259</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00346296296296296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00438283564814815</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00361657407407407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00437268518518518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="112416216"/>
+        <c:axId val="112413160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="602453896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112410248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="112410248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="602453896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="112413160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112416216"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="112416216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112413160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRF Iterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$G$3:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>123.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>175.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>251.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>291.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>287.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>318.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>168.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>253.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>294.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>264.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>301.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="602406440"/>
+        <c:axId val="602403144"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$A$3:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Feature Selection Batch CRF Fin'!$F$3:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.00146412037037037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00226041666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00227893518518518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00340509259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00409953703703704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00388541666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00425231481481481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00234259259259259</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00346296296296296</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00438283564814815</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.00361657407407407</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.00437268518518518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="112573544"/>
+        <c:axId val="602400104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="112573544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="602400104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="602400104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="h:mm;@" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="112573544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="602403144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="602406440"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="602406440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="602403144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -771,6 +3046,174 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1101,10 +3544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1112,43 +3555,47 @@
     <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>6</v>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2">
         <v>0.01</v>
       </c>
@@ -1165,15 +3612,21 @@
         <v>0.56903141605295104</v>
       </c>
       <c r="F3" s="3">
-        <v>3.123587962962963E-3</v>
-      </c>
-      <c r="G3" s="6"/>
+        <v>2.9755092592592593E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>80</v>
+      </c>
       <c r="H3" s="1">
         <f>E3-MAX(E3:E14)</f>
         <v>-0.12020469505816</v>
       </c>
+      <c r="I3" s="1">
+        <f>E3-E14</f>
+        <v>-0.11151813894575291</v>
+      </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="2">
         <v>0.05</v>
       </c>
@@ -1190,15 +3643,21 @@
         <v>0.63438431655976102</v>
       </c>
       <c r="F4" s="3">
-        <v>3.4589814814814817E-3</v>
-      </c>
-      <c r="G4" s="6"/>
+        <v>2.9812384259259254E-3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>76</v>
+      </c>
       <c r="H4" s="1">
         <f>E4-MAX(E3:E14)</f>
         <v>-5.485179455135003E-2</v>
       </c>
+      <c r="I4" s="1">
+        <f>E4-E14</f>
+        <v>-4.6165238438942935E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>0.1</v>
       </c>
@@ -1215,15 +3674,21 @@
         <v>0.66672508982560696</v>
       </c>
       <c r="F5" s="3">
-        <v>9.7263310185185178E-3</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>8.3912499999999994E-3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>223</v>
+      </c>
       <c r="H5" s="1">
         <f>E5-MAX(E3:E14)</f>
         <v>-2.2511021285504085E-2</v>
       </c>
+      <c r="I5" s="1">
+        <f>E5-E14</f>
+        <v>-1.3824465173096989E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="2">
         <v>0.2</v>
       </c>
@@ -1240,15 +3705,21 @@
         <v>0.68063646639422604</v>
       </c>
       <c r="F6" s="3">
-        <v>1.2094201388888887E-2</v>
-      </c>
-      <c r="G6" s="6"/>
+        <v>1.1502800925925927E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>273</v>
+      </c>
       <c r="H6" s="1">
         <f>E6-MAX(E3:E14)</f>
         <v>-8.5996447168850132E-3</v>
       </c>
+      <c r="I6" s="1">
+        <f>E6-E14</f>
+        <v>8.691139552208238E-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="2">
         <v>0.3</v>
       </c>
@@ -1265,15 +3736,21 @@
         <v>0.68287563407381502</v>
       </c>
       <c r="F7" s="3">
-        <v>1.2925763888888888E-2</v>
-      </c>
-      <c r="G7" s="6"/>
+        <v>1.312951388888889E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>293</v>
+      </c>
       <c r="H7" s="1">
         <f>E7-MAX(E3:E14)</f>
         <v>-6.3604770372960306E-3</v>
       </c>
+      <c r="I7" s="1">
+        <f>E7-E14</f>
+        <v>2.3260790751110649E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>0.4</v>
       </c>
@@ -1290,15 +3767,21 @@
         <v>0.68851316018825204</v>
       </c>
       <c r="F8" s="3">
-        <v>1.231289351851852E-2</v>
-      </c>
-      <c r="G8" s="6"/>
+        <v>1.1546435185185187E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>276</v>
+      </c>
       <c r="H8" s="1">
         <f>E8-MAX(E3:E14)</f>
         <v>-7.2295092285901141E-4</v>
       </c>
+      <c r="I8" s="1">
+        <f>E8-E14</f>
+        <v>7.9636051895480842E-3</v>
+      </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
@@ -1315,15 +3798,21 @@
         <v>0.68365843086259204</v>
       </c>
       <c r="F9" s="3">
-        <v>1.1816365740740742E-2</v>
-      </c>
-      <c r="G9" s="6"/>
+        <v>1.0171747685185185E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>262</v>
+      </c>
       <c r="H9" s="1">
         <f>E9-MAX(E3:E14)</f>
         <v>-5.5776802485190125E-3</v>
       </c>
+      <c r="I9" s="1">
+        <f>E9-E14</f>
+        <v>3.1088758638880831E-3</v>
+      </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
         <v>0.6</v>
       </c>
@@ -1340,15 +3829,21 @@
         <v>0.68522855408101302</v>
       </c>
       <c r="F10" s="3">
-        <v>1.1684687499999999E-2</v>
-      </c>
-      <c r="G10" s="6"/>
+        <v>1.0347245370370369E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>253</v>
+      </c>
       <c r="H10" s="1">
         <f>E10-MAX(E3:E14)</f>
         <v>-4.0075570300980301E-3</v>
       </c>
+      <c r="I10" s="1">
+        <f>E10-E14</f>
+        <v>4.6789990823090655E-3</v>
+      </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="2">
         <v>0.7</v>
       </c>
@@ -1365,15 +3860,20 @@
         <v>0.68923611111111105</v>
       </c>
       <c r="F11" s="3">
-        <v>1.2285717592592593E-2</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="1">
-        <f>E11-MAX(E3:E14)</f>
-        <v>0</v>
+        <v>1.0869722222222223E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>271</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1">
+        <f>E11-E14</f>
+        <v>8.6865561124070956E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="2">
         <v>0.8</v>
       </c>
@@ -1392,13 +3892,19 @@
       <c r="F12" s="3">
         <v>9.402337962962963E-3</v>
       </c>
-      <c r="G12" s="6"/>
+      <c r="G12" s="5">
+        <v>198</v>
+      </c>
       <c r="H12" s="1">
         <f>E12-MAX(E3:E14)</f>
         <v>-5.9071169255690004E-3</v>
       </c>
+      <c r="I12" s="1">
+        <f>E12-E14</f>
+        <v>2.7794391868380952E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="2">
         <v>0.9</v>
       </c>
@@ -1417,13 +3923,19 @@
       <c r="F13" s="3">
         <v>9.7779745370370364E-3</v>
       </c>
-      <c r="G13" s="6"/>
+      <c r="G13" s="5">
+        <v>226</v>
+      </c>
       <c r="H13" s="1">
         <f>E13-MAX(E3:E14)</f>
         <v>-4.2330647189100512E-3</v>
       </c>
+      <c r="I13" s="1">
+        <f>E13-E14</f>
+        <v>4.4534913934970444E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="2">
         <v>1</v>
       </c>
@@ -1442,15 +3954,18 @@
       <c r="F14" s="3">
         <v>9.1535300925925916E-3</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>203</v>
       </c>
       <c r="H14" s="1">
         <f>E14-MAX(E3:E14)</f>
         <v>-8.6865561124070956E-3</v>
       </c>
+      <c r="I14" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="E15" s="1"/>
     </row>
   </sheetData>
@@ -1458,7 +3973,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E14">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1470,6 +3985,550 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H10 H12:H14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B3">
+        <v>460</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.63002524762089696</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.53779840848806404</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.58027010106430599</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.3232870370370369E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>60</v>
+      </c>
+      <c r="H3" s="1">
+        <f>E3-MAX(E3:E14)</f>
+        <v>-0.11023094277703005</v>
+      </c>
+      <c r="I3" s="1">
+        <f>E3-E14</f>
+        <v>-0.10986341722943405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="B4">
+        <v>2303</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.70182868142444699</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.60444297082228104</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.64950565600783805</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3.6501504629629631E-3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>164</v>
+      </c>
+      <c r="H4" s="1">
+        <f>E4-MAX(E3:E14)</f>
+        <v>-4.0995387833497987E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <f>E4-E14</f>
+        <v>-4.0627862285901983E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>4607</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.71335927367055796</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.63826259946949604</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.67372473532242505</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4.8137268518518512E-3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>213</v>
+      </c>
+      <c r="H5" s="1">
+        <f>E5-MAX(E3:E14)</f>
+        <v>-1.6776308518910987E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f>E5-E14</f>
+        <v>-1.6408782971314984E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>9214</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.72077562326869804</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.64704907161803704</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.68192539530007901</v>
+      </c>
+      <c r="F6" s="3">
+        <v>6.3514351851851848E-3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>281</v>
+      </c>
+      <c r="H6" s="1">
+        <f>E6-MAX(E3:E14)</f>
+        <v>-8.5756485412570305E-3</v>
+      </c>
+      <c r="I6" s="1">
+        <f>E6-E14</f>
+        <v>-8.2081229936610267E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>13821</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.72365428354814298</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.63295755968169798</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.67527414220021198</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2.7813194444444443E-3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>101</v>
+      </c>
+      <c r="H7" s="1">
+        <f>E7-MAX(E3:E14)</f>
+        <v>-1.5226901641124058E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <f>E7-E14</f>
+        <v>-1.4859376093528054E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>18428</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.72602230483271402</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.64754641909814303</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.68454258675078905</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5.3487268518518519E-3</v>
+      </c>
+      <c r="G8" s="5">
+        <v>222</v>
+      </c>
+      <c r="H8" s="1">
+        <f>E8-MAX(E3:E14)</f>
+        <v>-5.9584570905469869E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <f>E8-E14</f>
+        <v>-5.5909315429509832E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>23035</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.72239516572056395</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.65401193633952304</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.68650482902636401</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7.1733101851851853E-3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>297</v>
+      </c>
+      <c r="H9" s="1">
+        <f>E9-MAX(E3:E14)</f>
+        <v>-3.9962148149720322E-3</v>
+      </c>
+      <c r="I9" s="1">
+        <f>E9-E14</f>
+        <v>-3.6286892673760285E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>27642</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.71648830038091804</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.65484084880636595</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.68427890861844998</v>
+      </c>
+      <c r="F10" s="3">
+        <v>6.0759953703703705E-3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>249</v>
+      </c>
+      <c r="H10" s="1">
+        <f>E10-MAX(E3:E14)</f>
+        <v>-6.2221352228860605E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <f>E10-E14</f>
+        <v>-5.8546096752900567E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>32249</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.72021296126308099</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.65036472148541102</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.68350901646484896</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5.5178472222222226E-3</v>
+      </c>
+      <c r="G11" s="5">
+        <v>217</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1">
+        <f>E11-E14</f>
+        <v>-6.6245018288910718E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>36856</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.72639092240117098</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.65799071618037097</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.69050104384133604</v>
+      </c>
+      <c r="F12" s="3">
+        <v>7.0165046296296295E-3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>282</v>
+      </c>
+      <c r="H12" s="1">
+        <f>E12-MAX(E3:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>E12-E14</f>
+        <v>3.6752554759600375E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="B13">
+        <v>41463</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.72122204037097704</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.65749336870026498</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.687884832191484</v>
+      </c>
+      <c r="F13" s="3">
+        <v>6.2756365740740741E-3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>245</v>
+      </c>
+      <c r="H13" s="1">
+        <f>E13-MAX(E3:E14)</f>
+        <v>-2.6162116498520405E-3</v>
+      </c>
+      <c r="I13" s="1">
+        <f>E13-E14</f>
+        <v>-2.2486861022560367E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>46071</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.72337331879316602</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.65981432360742698</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.69013351829374003</v>
+      </c>
+      <c r="F14" s="3">
+        <v>7.9270717592592587E-3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>332</v>
+      </c>
+      <c r="H14" s="1">
+        <f>E14-MAX(E3:E14)</f>
+        <v>-3.6752554759600375E-4</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="E15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E3:E14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:G14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H10 H12:H14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1481,7 +4540,528 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H14">
+  <conditionalFormatting sqref="I3:I13">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="B3">
+        <v>460</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.644159072</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.515583554</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.57274401500000005</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.4641203703703706E-3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>123</v>
+      </c>
+      <c r="H3" s="1">
+        <f>E3-MAX(E3:E14)</f>
+        <v>-0.11725423899999998</v>
+      </c>
+      <c r="I3" s="1">
+        <f>E3-E14</f>
+        <v>-0.11495042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="B4">
+        <v>2303</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.70025140200000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.60029840800000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.64643399099999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.2604166666666667E-3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>173</v>
+      </c>
+      <c r="H4" s="1">
+        <f>E4-MAX(E3:E14)</f>
+        <v>-4.3564263000000047E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <f>E4-E14</f>
+        <v>-4.1260444000000063E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <v>4607</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.70976744199999997</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.63246021200000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.66888752500000004</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2.2789351851851855E-3</v>
+      </c>
+      <c r="G5" s="5">
+        <v>175</v>
+      </c>
+      <c r="H5" s="1">
+        <f>E5-MAX(E3:E14)</f>
+        <v>-2.1110728999999995E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f>E5-E14</f>
+        <v>-1.880691000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>9214</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.71124173400000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.64190981400000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.67479958200000001</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3.4050925925925928E-3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>251</v>
+      </c>
+      <c r="H6" s="1">
+        <f>E6-MAX(E3:E14)</f>
+        <v>-1.5198672000000024E-2</v>
+      </c>
+      <c r="I6" s="1">
+        <f>E6-E14</f>
+        <v>-1.2894853000000039E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="B7">
+        <v>13821</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.72091310799999997</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.64920424399999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.68318213500000002</v>
+      </c>
+      <c r="F7" s="3">
+        <v>4.099537037037037E-3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>291</v>
+      </c>
+      <c r="H7" s="1">
+        <f>E7-MAX(E3:E14)</f>
+        <v>-6.8161190000000094E-3</v>
+      </c>
+      <c r="I7" s="1">
+        <f>E7-E14</f>
+        <v>-4.5123000000000246E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="B8">
+        <v>18428</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.72304011800000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.65135941600000002</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.68533054199999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3.8854166666666668E-3</v>
+      </c>
+      <c r="G8" s="5">
+        <v>287</v>
+      </c>
+      <c r="H8" s="1">
+        <f>E8-MAX(E3:E14)</f>
+        <v>-4.667712000000046E-3</v>
+      </c>
+      <c r="I8" s="1">
+        <f>E8-E14</f>
+        <v>-2.3638930000000613E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>23035</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.72852930299999996</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.65533819599999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.68999825400000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4.2523148148148147E-3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>318</v>
+      </c>
+      <c r="H9" s="1">
+        <f>E9-MAX(E3:E14)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f>E9-E14</f>
+        <v>2.3038189999999847E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="B10">
+        <v>27642</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.71413082800000005</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.65517241400000004</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.68338232799999998</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.3425925925925923E-3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>168</v>
+      </c>
+      <c r="H10" s="1">
+        <f>E10-MAX(E3:E14)</f>
+        <v>-6.6159260000000497E-3</v>
+      </c>
+      <c r="I10" s="1">
+        <f>E10-E14</f>
+        <v>-4.312107000000065E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="B11">
+        <v>32249</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.73041044799999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.64903846200000004</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.68732443799999998</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3.4629629629629628E-3</v>
+      </c>
+      <c r="G11" s="5">
+        <v>253</v>
+      </c>
+      <c r="H11" s="1">
+        <f>E11-MAX(E3:E14)</f>
+        <v>-2.673816000000051E-3</v>
+      </c>
+      <c r="I11" s="1">
+        <f>E11-E14</f>
+        <v>-3.699970000000663E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="B12">
+        <v>36856</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.727675276752768</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.65384615384615397</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.68878798463150503</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4.3828356481481479E-3</v>
+      </c>
+      <c r="G12" s="5">
+        <v>294</v>
+      </c>
+      <c r="H12" s="1">
+        <f>E12-MAX(E3:E14)</f>
+        <v>-1.2102693684949983E-3</v>
+      </c>
+      <c r="I12" s="1">
+        <f>E12-E14</f>
+        <v>1.0935496315049864E-3</v>
+      </c>
+      <c r="J12" s="8">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="B13">
+        <v>41463</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.71929190751445105</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.66014588859416401</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.688450899031812</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3.6165740740740741E-3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>264</v>
+      </c>
+      <c r="H13" s="1">
+        <f>E13-MAX(E3:E14)</f>
+        <v>-1.5473549681880305E-3</v>
+      </c>
+      <c r="I13" s="1">
+        <f>E13-E14</f>
+        <v>7.5646403181195421E-4</v>
+      </c>
+      <c r="J13" s="8">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>46071</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.71823104699999996</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.65964854100000003</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.68769443500000005</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.3726851851851852E-3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>301</v>
+      </c>
+      <c r="H14" s="1">
+        <f>E14-MAX(E3:E14)</f>
+        <v>-2.3038189999999847E-3</v>
+      </c>
+      <c r="I14" s="1">
+        <f>E14-E14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="E15" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E3:E14">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:G14">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H10 H12:H14">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F14">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G14">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>